<commit_message>
Finished first analysis, added 2021-22 games data
</commit_message>
<xml_diff>
--- a/Games Data Raw/Titans Games 2022.xlsx
+++ b/Games Data Raw/Titans Games 2022.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sovann\Git\NSC-Capstone\Games Data Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548D8EE5-C614-4ABD-8DB9-44EBDB8AD575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D55EF1-0375-4BD2-AC6D-E1A8AF1BFAA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="26537" windowHeight="15943" xr2:uid="{1E0A21F6-DDD8-4049-AAC6-E33E6092C5EC}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>